<commit_message>
add upload work order and list wok order
</commit_message>
<xml_diff>
--- a/assets/List Work Order 1.xlsx
+++ b/assets/List Work Order 1.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,31 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>Part Name</t>
-  </si>
-  <si>
-    <t>No Work Order</t>
-  </si>
-  <si>
-    <t>Customer</t>
-  </si>
-  <si>
-    <t>Prod Date</t>
-  </si>
-  <si>
-    <t>Quantity perbox</t>
-  </si>
-  <si>
-    <t>Total Order</t>
-  </si>
-  <si>
-    <t>Total Box</t>
-  </si>
-  <si>
-    <t>Supplier</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>GARNISH RR BUMPER LWR (IPL)</t>
   </si>
@@ -60,13 +37,43 @@
   </si>
   <si>
     <t>TKI</t>
+  </si>
+  <si>
+    <t>no_work _order</t>
+  </si>
+  <si>
+    <t>customer</t>
+  </si>
+  <si>
+    <t>prod_date</t>
+  </si>
+  <si>
+    <t>quantity_perbox</t>
+  </si>
+  <si>
+    <t>total_order</t>
+  </si>
+  <si>
+    <t>total_box</t>
+  </si>
+  <si>
+    <t>supplier</t>
+  </si>
+  <si>
+    <t>part_name</t>
+  </si>
+  <si>
+    <t>GARNISH RR BUMPER LWR (IPR)</t>
+  </si>
+  <si>
+    <t>no_work_order</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,6 +84,12 @@
     <font>
       <sz val="10"/>
       <color rgb="FF777777"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -104,10 +117,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -391,7 +402,7 @@
   <dimension ref="B2:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -407,41 +418,41 @@
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="I2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="3">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2">
         <v>44857</v>
       </c>
       <c r="F3" s="1">
@@ -454,11 +465,45 @@
         <v>90</v>
       </c>
       <c r="I3" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="58.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>